<commit_message>
updated & new functs
</commit_message>
<xml_diff>
--- a/16StatePolicies_details_March_1.xlsx
+++ b/16StatePolicies_details_March_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEGA\IDEA\YEAR 2\EXTRA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEGA\IDEA\YEAR 2\EXTRA\Codes - Ivana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A856A0-5725-42AD-93E0-F04D5F646F0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE7B4D4-8743-4DA0-91F6-1CB209C4C2A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B5ADD841-D026-4197-8972-43813B08C1FA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="106">
   <si>
     <t>No</t>
   </si>
@@ -360,6 +360,45 @@
   </si>
   <si>
     <t>Binary variable, takes a value of 1 when restrictions on traveling to the state are present in some form.</t>
+  </si>
+  <si>
+    <t>Type of Var (by values it takes)</t>
+  </si>
+  <si>
+    <t>bin</t>
+  </si>
+  <si>
+    <t>cat_sch</t>
+  </si>
+  <si>
+    <t>cat_bus</t>
+  </si>
+  <si>
+    <t>numb</t>
+  </si>
+  <si>
+    <t>cat_mand</t>
+  </si>
+  <si>
+    <t>bin_rec</t>
+  </si>
+  <si>
+    <t>Usual no-restrictiions value</t>
+  </si>
+  <si>
+    <t>InPersonAllowed</t>
+  </si>
+  <si>
+    <t>IndoorAllowed</t>
+  </si>
+  <si>
+    <t>999999 (no max)</t>
+  </si>
+  <si>
+    <t>NotMentioned</t>
+  </si>
+  <si>
+    <t>VaccineExempt</t>
   </si>
 </sst>
 </file>
@@ -512,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -556,9 +595,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -614,6 +650,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -930,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E210DAD-944D-4067-BAB7-0306D0393778}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,10 +990,14 @@
     <col min="8" max="8" width="21.109375" style="3" customWidth="1"/>
     <col min="9" max="9" width="18.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.33203125" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="3"/>
+    <col min="11" max="11" width="16.77734375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="3"/>
+    <col min="14" max="14" width="22.109375" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -982,72 +1028,93 @@
       <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" s="33" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="31">
+    <row r="2" spans="1:14" s="32" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="30">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="32" t="s">
         <v>18</v>
       </c>
+      <c r="K2" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" s="32">
+        <v>0</v>
+      </c>
+      <c r="N2" s="35" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" s="18" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
+    <row r="3" spans="1:14" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="18" t="s">
+      <c r="C3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="K3" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -1066,8 +1133,8 @@
       <c r="F4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>0</v>
+      <c r="G4" s="29" t="s">
+        <v>21</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>42</v>
@@ -1078,8 +1145,14 @@
       <c r="J4" s="14" t="s">
         <v>41</v>
       </c>
+      <c r="K4" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1098,8 +1171,8 @@
       <c r="F5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>0</v>
+      <c r="G5" s="34" t="s">
+        <v>21</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>43</v>
@@ -1110,8 +1183,14 @@
       <c r="J5" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="K5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1130,8 +1209,8 @@
       <c r="F6" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="15" t="s">
-        <v>0</v>
+      <c r="G6" s="29" t="s">
+        <v>21</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>44</v>
@@ -1142,40 +1221,52 @@
       <c r="J6" s="14" t="s">
         <v>41</v>
       </c>
+      <c r="K6" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" s="18" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+    <row r="7" spans="1:14" s="17" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
         <v>6</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="18" t="s">
+      <c r="D7" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="18" t="s">
+      <c r="G7" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="17" t="s">
         <v>41</v>
       </c>
+      <c r="K7" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1206,8 +1297,14 @@
       <c r="J8" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="K8" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1238,8 +1335,14 @@
       <c r="J9" s="4" t="s">
         <v>61</v>
       </c>
+      <c r="K9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1270,73 +1373,91 @@
       <c r="J10" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="K10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="26">
+    <row r="11" spans="1:14" s="20" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
         <v>10</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="21" t="s">
+      <c r="C11" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="21" t="s">
+      <c r="G11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="20" t="s">
         <v>73</v>
       </c>
+      <c r="K11" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="L11" s="20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" s="24" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
+    <row r="12" spans="1:14" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="26">
         <v>11</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="24" t="s">
+      <c r="D12" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" s="24" t="s">
+      <c r="G12" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="23" t="s">
         <v>72</v>
       </c>
+      <c r="K12" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="L12" s="23">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="28">
+    <row r="13" spans="1:14" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="27">
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -1366,9 +1487,15 @@
       <c r="J13" s="4" t="s">
         <v>76</v>
       </c>
+      <c r="K13" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="29">
+    <row r="14" spans="1:14" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="28">
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -1398,41 +1525,53 @@
       <c r="J14" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="K14" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" s="18" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="16">
+    <row r="15" spans="1:14" s="17" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="15">
         <v>14</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="18" t="s">
+      <c r="D15" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="G15" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="18" t="s">
+      <c r="G15" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="I15" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="J15" s="18" t="s">
+      <c r="J15" s="17" t="s">
         <v>41</v>
       </c>
+      <c r="K15" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="29">
+    <row r="16" spans="1:14" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="28">
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -1462,9 +1601,15 @@
       <c r="J16" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="K16" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="28">
+    <row r="17" spans="1:12" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="27">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -1493,9 +1638,16 @@
       </c>
       <c r="J17" s="4" t="s">
         <v>92</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed & updated functs
</commit_message>
<xml_diff>
--- a/16StatePolicies_details_March_1.xlsx
+++ b/16StatePolicies_details_March_1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEGA\IDEA\YEAR 2\EXTRA\Codes - Ivana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE7B4D4-8743-4DA0-91F6-1CB209C4C2A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADFD73C-B56E-4FF6-8557-B8AAAE92E263}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B5ADD841-D026-4197-8972-43813B08C1FA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B5ADD841-D026-4197-8972-43813B08C1FA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ref" sheetId="1" r:id="rId1"/>
+    <sheet name="working on" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="138">
   <si>
     <t>No</t>
   </si>
@@ -254,9 +255,6 @@
     <t>StayAtHome.R</t>
   </si>
   <si>
-    <t>Categorical variable, three levels possible: Mandatory &gt; Recommended &gt; NotMentioned</t>
-  </si>
-  <si>
     <t>AppliesTo; Mandate; PolicyNotes; PublicMaskLevel</t>
   </si>
   <si>
@@ -380,9 +378,6 @@
     <t>cat_mand</t>
   </si>
   <si>
-    <t>bin_rec</t>
-  </si>
-  <si>
     <t>Usual no-restrictiions value</t>
   </si>
   <si>
@@ -398,14 +393,116 @@
     <t>NotMentioned</t>
   </si>
   <si>
-    <t>VaccineExempt</t>
+    <t>To do:</t>
+  </si>
+  <si>
+    <t>location specified + Ends = Leaves</t>
+  </si>
+  <si>
+    <t>View(filter(COVID_measures_df_REVIEWED, !(is.na(Leaves)) &amp; !(is.na(Ends))))</t>
+  </si>
+  <si>
+    <t>one instance where both leaves and ends are present in the whole df</t>
+  </si>
+  <si>
+    <t>AppliesTo - states instead of counties</t>
+  </si>
+  <si>
+    <t>Finish the FILL function</t>
+  </si>
+  <si>
+    <t>step 1 - fill for the first policy entry regarding the policy chain</t>
+  </si>
+  <si>
+    <t>perc_usual_time</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>groups (vaccinated vs. not)</t>
+  </si>
+  <si>
+    <t>limits gatherinings</t>
+  </si>
+  <si>
+    <t>mandate</t>
+  </si>
+  <si>
+    <t>policy_measure_var_main</t>
+  </si>
+  <si>
+    <t>policy_measure_var_sec</t>
+  </si>
+  <si>
+    <t>make NA</t>
+  </si>
+  <si>
+    <t>(both are date-location dependent)</t>
+  </si>
+  <si>
+    <t>step 2 - fill for the first policy entry regarding the policy chain VALUES</t>
+  </si>
+  <si>
+    <t>step 3 - fill for the remaining policy entries within this policy/state df</t>
+  </si>
+  <si>
+    <t>Note to self</t>
+  </si>
+  <si>
+    <t>Expands / Eases</t>
+  </si>
+  <si>
+    <t>policy value changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leaves / Joins </t>
+  </si>
+  <si>
+    <t>related to location</t>
+  </si>
+  <si>
+    <t>same thing for Ease/Expand + Location</t>
+  </si>
+  <si>
+    <t>259/2507 cases of Leaves/Joins have no applies to argument</t>
+  </si>
+  <si>
+    <t>Extract Values from</t>
+  </si>
+  <si>
+    <t>SchoolRestrictLevel</t>
+  </si>
+  <si>
+    <t>BusinessRestrictLevel</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Categorical variable, 2 levels possible: Mandatory &gt; Recommended</t>
+  </si>
+  <si>
+    <t>re-save the environment up until EELJ</t>
+  </si>
+  <si>
+    <t>SWPop check</t>
+  </si>
+  <si>
+    <t>no change detected</t>
+  </si>
+  <si>
+    <t>easing example of CaseIsolation in Alabama</t>
+  </si>
+  <si>
+    <t>change mandatory to 0.5?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,8 +564,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF9D00"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -502,6 +613,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,7 +668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -658,6 +775,32 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -974,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E210DAD-944D-4067-BAB7-0306D0393778}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -992,7 +1135,7 @@
     <col min="10" max="10" width="25.33203125" style="3" customWidth="1"/>
     <col min="11" max="11" width="16.77734375" style="3" customWidth="1"/>
     <col min="12" max="12" width="17.88671875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="3"/>
+    <col min="13" max="13" width="19.44140625" style="3" customWidth="1"/>
     <col min="14" max="14" width="22.109375" style="3" customWidth="1"/>
     <col min="15" max="16384" width="8.88671875" style="3"/>
   </cols>
@@ -1029,10 +1172,13 @@
         <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="32" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -1067,14 +1213,15 @@
         <v>18</v>
       </c>
       <c r="K2" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L2" s="32">
         <v>0</v>
       </c>
-      <c r="N2" s="35" t="s">
-        <v>105</v>
-      </c>
+      <c r="M2" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="N2" s="35"/>
     </row>
     <row r="3" spans="1:14" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
@@ -1108,10 +1255,13 @@
         <v>24</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -1128,7 +1278,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>26</v>
@@ -1146,10 +1296,13 @@
         <v>41</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -1184,10 +1337,13 @@
         <v>47</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -1204,7 +1360,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>49</v>
@@ -1222,10 +1378,13 @@
         <v>41</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="17" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -1242,7 +1401,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>50</v>
@@ -1260,10 +1419,13 @@
         <v>41</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -1298,10 +1460,13 @@
         <v>57</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L8" s="2">
         <v>0</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -1333,13 +1498,16 @@
         <v>31</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>61</v>
+        <v>132</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>104</v>
+        <v>93</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -1356,28 +1524,28 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>32</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="20" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -1397,25 +1565,28 @@
         <v>58</v>
       </c>
       <c r="F11" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="20" t="s">
         <v>67</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>68</v>
       </c>
       <c r="I11" s="20" t="s">
         <v>33</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L11" s="20">
         <v>0</v>
+      </c>
+      <c r="M11" s="20" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -1426,7 +1597,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>0</v>
@@ -1435,25 +1606,28 @@
         <v>58</v>
       </c>
       <c r="F12" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="23" t="s">
         <v>70</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>71</v>
       </c>
       <c r="I12" s="23" t="s">
         <v>34</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L12" s="23">
         <v>0</v>
+      </c>
+      <c r="M12" s="23" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -1473,25 +1647,28 @@
         <v>58</v>
       </c>
       <c r="F13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>35</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L13" s="4">
         <v>0</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -1508,28 +1685,31 @@
         <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>36</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L14" s="2">
         <v>0</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="17" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -1546,28 +1726,31 @@
         <v>0</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F15" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="G15" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>83</v>
-      </c>
       <c r="I15" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J15" s="17" t="s">
         <v>41</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="M15" s="17" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -1578,37 +1761,40 @@
         <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="G16" s="10" t="s">
         <v>0</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>38</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L16" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="M16" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="27">
         <v>16</v>
       </c>
@@ -1616,34 +1802,244 @@
         <v>39</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>39</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K17" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{028F7423-37BC-4E43-B0A9-8D7586E6446A}">
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" style="38" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" style="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.21875" style="37" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" style="37" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25" style="38" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="37"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="36">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C3" s="40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="36">
+        <v>2</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="36">
+        <v>3</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C7" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D8" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="L17" s="4">
-        <v>0</v>
+      <c r="E8" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="38"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D9" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="38"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D10" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="38"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D11" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="38"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D12" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="38"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E13" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="38"/>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C15" s="38" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="38" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C21" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="36">
+        <v>4</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="36">
+        <v>5</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="37" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improvements and additional functions
Changes, up to 27/05.
</commit_message>
<xml_diff>
--- a/16StatePolicies_details_March_1.xlsx
+++ b/16StatePolicies_details_March_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEGA\IDEA\YEAR 2\EXTRA\Codes - Ivana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45D9992-0C2D-46FE-9390-E456AC6098C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7638B04B-C08D-42A2-88D4-6AAA63D06DED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B5ADD841-D026-4197-8972-43813B08C1FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="147">
   <si>
     <t>No</t>
   </si>
@@ -511,6 +511,18 @@
   </si>
   <si>
     <t>check for ch_uncoded cases</t>
+  </si>
+  <si>
+    <t>re-do the plot function</t>
+  </si>
+  <si>
+    <t>based on the dimension (mandate filtering etc.)</t>
+  </si>
+  <si>
+    <t>x-axis: time, y-axis policy measure vale</t>
+  </si>
+  <si>
+    <t>interpolation after filtering</t>
   </si>
 </sst>
 </file>
@@ -692,7 +704,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -721,12 +733,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -745,25 +751,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -828,6 +825,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1144,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E210DAD-944D-4067-BAB7-0306D0393778}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1208,127 +1235,127 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="32" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="30">
+    <row r="2" spans="1:14" s="27" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="L2" s="32">
-        <v>0</v>
-      </c>
-      <c r="M2" s="32" t="s">
+      <c r="L2" s="27">
+        <v>0</v>
+      </c>
+      <c r="M2" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="N2" s="35"/>
-    </row>
-    <row r="3" spans="1:14" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="15">
+      <c r="N2" s="30"/>
+    </row>
+    <row r="3" spans="1:14" s="15" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="17" t="s">
+      <c r="C3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+    <row r="4" spans="1:14" s="12" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M4" s="12" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1351,10 +1378,10 @@
       <c r="F5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="49" t="s">
         <v>43</v>
       </c>
       <c r="I5" s="4" t="s">
@@ -1373,85 +1400,85 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
+    <row r="6" spans="1:14" s="12" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="14" t="s">
+      <c r="D6" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="17" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="15">
+    <row r="7" spans="1:14" s="15" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="M7" s="17" t="s">
+      <c r="M7" s="15" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1474,10 +1501,10 @@
       <c r="F8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="G8" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="50" t="s">
         <v>56</v>
       </c>
       <c r="I8" s="2" t="s">
@@ -1515,10 +1542,10 @@
       <c r="F9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="G9" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="49" t="s">
         <v>60</v>
       </c>
       <c r="I9" s="4" t="s">
@@ -1556,10 +1583,10 @@
       <c r="F10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="G10" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="50" t="s">
         <v>63</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -1575,90 +1602,90 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="20" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="25">
+    <row r="11" spans="1:14" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="20">
         <v>10</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="20" t="s">
+      <c r="C11" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="20" t="s">
+      <c r="G11" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="K11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="L11" s="20">
-        <v>0</v>
-      </c>
-      <c r="M11" s="20" t="s">
+      <c r="L11" s="17">
+        <v>0</v>
+      </c>
+      <c r="M11" s="17" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="26">
+    <row r="12" spans="1:14" s="19" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="21">
         <v>11</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="23" t="s">
+      <c r="D12" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" s="23" t="s">
+      <c r="G12" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="K12" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="L12" s="23">
-        <v>0</v>
-      </c>
-      <c r="M12" s="23" t="s">
+      <c r="L12" s="19">
+        <v>0</v>
+      </c>
+      <c r="M12" s="19" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="27">
+      <c r="A13" s="22">
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -1676,10 +1703,10 @@
       <c r="F13" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" s="4" t="s">
+      <c r="G13" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="49" t="s">
         <v>74</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -1699,7 +1726,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="28">
+      <c r="A14" s="23">
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -1717,10 +1744,10 @@
       <c r="F14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G14" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2" t="s">
+      <c r="G14" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="50" t="s">
         <v>78</v>
       </c>
       <c r="I14" s="2" t="s">
@@ -1739,49 +1766,49 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="17" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="15">
+    <row r="15" spans="1:14" s="15" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="13">
         <v>14</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="17" t="s">
+      <c r="D15" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="17" t="s">
+      <c r="G15" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="J15" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="K15" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="L15" s="17" t="s">
+      <c r="L15" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="M15" s="17" t="s">
+      <c r="M15" s="15" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="28">
+      <c r="A16" s="23">
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -1799,10 +1826,10 @@
       <c r="F16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="G16" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="50" t="s">
         <v>79</v>
       </c>
       <c r="I16" s="2" t="s">
@@ -1822,7 +1849,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="27">
+      <c r="A17" s="22">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -1840,10 +1867,10 @@
       <c r="F17" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G17" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4" t="s">
+      <c r="G17" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="49" t="s">
         <v>90</v>
       </c>
       <c r="I17" s="4" t="s">
@@ -1870,292 +1897,309 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{028F7423-37BC-4E43-B0A9-8D7586E6446A}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.77734375" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" style="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23" style="37" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.21875" style="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25" style="38" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="37"/>
+    <col min="1" max="1" width="2" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" style="33" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" style="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.21875" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25" style="33" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="31" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="36">
+      <c r="A2" s="31">
         <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="I2" s="37" t="s">
+      <c r="I2" s="32" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="35" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="36">
+      <c r="A4" s="31">
         <v>2</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="32" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="36">
+      <c r="A5" s="31">
         <v>3</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="36" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="F7" s="40" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="F8" s="38"/>
+      <c r="F8" s="33"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="F9" s="38"/>
+      <c r="F9" s="33"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="F10" s="38"/>
+      <c r="F10" s="33"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="F11" s="38"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="F12" s="38"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="F13" s="38"/>
+      <c r="F13" s="33"/>
     </row>
     <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="E15" s="44" t="s">
+      <c r="E15" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="F15" s="45" t="s">
+      <c r="F15" s="40" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="F16" s="38"/>
+      <c r="F16" s="33"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D17" s="47" t="s">
+      <c r="D17" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="E17" s="47" t="s">
+      <c r="E17" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="F17" s="38"/>
+      <c r="F17" s="33"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D18" s="47" t="s">
+      <c r="D18" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E18" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="33"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D19" s="47" t="s">
+      <c r="D19" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="E19" s="47" t="s">
+      <c r="E19" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="F19" s="38"/>
+      <c r="F19" s="33"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D20" s="48" t="s">
+      <c r="D20" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="47" t="s">
+      <c r="E20" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="F20" s="38"/>
+      <c r="F20" s="33"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D21" s="47"/>
-      <c r="E21" s="47" t="s">
+      <c r="D21" s="42"/>
+      <c r="E21" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="F21" s="38"/>
+      <c r="F21" s="33"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="33" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="32" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="32" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="36">
+      <c r="A25" s="31">
         <v>4</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="32" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="36">
+      <c r="A26" s="31">
         <v>5</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="32" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="36">
+      <c r="A27" s="31">
         <v>6</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="33" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="36">
+      <c r="A28" s="31">
         <v>7</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="C28" s="38" t="s">
+      <c r="C28" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="D28" s="50" t="s">
+      <c r="D28" s="45" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="31">
+        <v>8</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last updates of data frames, mid-June
</commit_message>
<xml_diff>
--- a/16StatePolicies_details_March_1.xlsx
+++ b/16StatePolicies_details_March_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEGA\IDEA\YEAR 2\EXTRA\SocialDistancingDataManipulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993FA6AB-0C95-47C5-B77F-973636FA4183}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6844D3E-F932-4C22-85F0-2E79CDF7A6CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B5ADD841-D026-4197-8972-43813B08C1FA}"/>
   </bookViews>
@@ -615,7 +615,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,12 +631,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -698,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -706,18 +700,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -727,25 +712,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -759,55 +729,49 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1126,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E210DAD-944D-4067-BAB7-0306D0393778}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1150,7 +1114,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1190,657 +1154,657 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="11">
+    <row r="2" spans="1:14" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="L2" s="13">
-        <v>0</v>
-      </c>
-      <c r="M2" s="13" t="s">
+      <c r="L2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="N2" s="16"/>
-    </row>
-    <row r="3" spans="1:14" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="13" t="s">
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="38" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="36">
+    <row r="4" spans="1:14" s="28" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="26">
         <v>3</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="38" t="s">
+      <c r="D4" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="J4" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="L4" s="38" t="s">
+      <c r="L4" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="M4" s="38" t="s">
+      <c r="M4" s="28" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+    <row r="5" spans="1:14" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="C5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="38" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" s="36">
+    <row r="6" spans="1:14" s="28" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="26">
         <v>5</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="38" t="s">
+      <c r="D6" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="J6" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="K6" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="L6" s="38" t="s">
+      <c r="L6" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="M6" s="28" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="9" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+    <row r="7" spans="1:14" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="D7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="M7" s="6" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="38" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="36">
+    <row r="8" spans="1:14" s="28" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="26">
         <v>7</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="40" t="s">
+      <c r="H8" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="38" t="s">
+      <c r="I8" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="38" t="s">
+      <c r="J8" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="37" t="s">
+      <c r="K8" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="L8" s="38">
-        <v>0</v>
-      </c>
-      <c r="M8" s="38" t="s">
+      <c r="L8" s="28">
+        <v>0</v>
+      </c>
+      <c r="M8" s="28" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
+    <row r="9" spans="1:14" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="13" t="s">
+      <c r="C9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="L9" s="13">
-        <v>0</v>
-      </c>
-      <c r="M9" s="13" t="s">
+      <c r="L9" s="6">
+        <v>0</v>
+      </c>
+      <c r="M9" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="38" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="36">
+    <row r="10" spans="1:14" s="28" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="26">
         <v>9</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="38" t="s">
+      <c r="C10" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="H10" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="38" t="s">
+      <c r="I10" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="38" t="s">
+      <c r="J10" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="K10" s="38" t="s">
+      <c r="K10" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="L10" s="38" t="s">
+      <c r="L10" s="28" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="41">
+    <row r="11" spans="1:14" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="31">
         <v>10</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="13" t="s">
+      <c r="C11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="L11" s="13">
-        <v>0</v>
-      </c>
-      <c r="M11" s="13" t="s">
+      <c r="L11" s="6">
+        <v>0</v>
+      </c>
+      <c r="M11" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="38" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="42">
+    <row r="12" spans="1:14" s="28" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="32">
         <v>11</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="38" t="s">
+      <c r="D12" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="40" t="s">
+      <c r="H12" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="38" t="s">
+      <c r="I12" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="38" t="s">
+      <c r="J12" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="K12" s="37" t="s">
+      <c r="K12" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="L12" s="38">
-        <v>0</v>
-      </c>
-      <c r="M12" s="38" t="s">
+      <c r="L12" s="28">
+        <v>0</v>
+      </c>
+      <c r="M12" s="28" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="41">
+    <row r="13" spans="1:14" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="31">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="13" t="s">
+      <c r="C13" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G13" s="35" t="s">
+      <c r="G13" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="32" t="s">
+      <c r="H13" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="K13" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="L13" s="13">
-        <v>0</v>
-      </c>
-      <c r="M13" s="13" t="s">
+      <c r="L13" s="6">
+        <v>0</v>
+      </c>
+      <c r="M13" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="38" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="42">
+    <row r="14" spans="1:14" s="28" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="32">
         <v>13</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="38" t="s">
+      <c r="C14" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="F14" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="G14" s="39" t="s">
+      <c r="G14" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="40" t="s">
+      <c r="H14" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="I14" s="38" t="s">
+      <c r="I14" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J14" s="38" t="s">
+      <c r="J14" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="K14" s="37" t="s">
+      <c r="K14" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="L14" s="38">
-        <v>0</v>
-      </c>
-      <c r="M14" s="38" t="s">
+      <c r="L14" s="28">
+        <v>0</v>
+      </c>
+      <c r="M14" s="28" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="9" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
+    <row r="15" spans="1:14" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="9" t="s">
+      <c r="D15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="H15" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="J15" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="L15" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="M15" s="9" t="s">
+      <c r="M15" s="6" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="38" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="42">
+    <row r="16" spans="1:14" s="28" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="32">
         <v>15</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F16" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G16" s="39" t="s">
+      <c r="G16" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="38" t="s">
+      <c r="J16" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="K16" s="37" t="s">
+      <c r="K16" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="L16" s="38">
-        <v>0</v>
-      </c>
-      <c r="M16" s="38" t="s">
+      <c r="L16" s="28">
+        <v>0</v>
+      </c>
+      <c r="M16" s="28" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="41">
+    <row r="17" spans="1:13" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="31">
         <v>16</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="G17" s="35" t="s">
+      <c r="G17" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="32" t="s">
+      <c r="H17" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="13" t="s">
+      <c r="J17" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="L17" s="13">
-        <v>0</v>
-      </c>
-      <c r="M17" s="13" t="s">
+      <c r="L17" s="6">
+        <v>0</v>
+      </c>
+      <c r="M17" s="6" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1860,300 +1824,300 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.77734375" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" style="19" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.21875" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25" style="19" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="18"/>
+    <col min="1" max="1" width="2" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.21875" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="9" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="17">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="13" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="17">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="10" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="17">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="14" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="18" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="F10" s="19"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="F12" s="19"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="F13" s="19"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="18" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="F16" s="19"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="F17" s="19"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="F18" s="19"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="F19" s="19"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="F20" s="19"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D21" s="28"/>
-      <c r="E21" s="28" t="s">
+      <c r="D21" s="20"/>
+      <c r="E21" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="11" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="10" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="10" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="17">
+      <c r="A25" s="9">
         <v>4</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="10" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="17">
+      <c r="A26" s="9">
         <v>5</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="10" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="17">
+      <c r="A27" s="9">
         <v>6</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="11" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="17">
+      <c r="A28" s="9">
         <v>7</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="23" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="17">
+      <c r="A29" s="9">
         <v>8</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="F29" s="18" t="s">
+      <c r="F29" s="10" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>